<commit_message>
docs: update metrics doc
</commit_message>
<xml_diff>
--- a/docs/FGW metrics说明.xlsx
+++ b/docs/FGW metrics说明.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linyang/SynologyDrive/Flomesh/001-内部资料/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4688EF-8F38-7E43-B11F-A666D48140D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743C8DE5-4DE7-5B4A-ACBC-FB7391BA4B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10140" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{0C346885-EE02-774F-9E3C-899FFF5F6B1C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="83">
   <si>
     <t>fgw_upstream_rq_retry</t>
   </si>
@@ -272,6 +272,18 @@
   </si>
   <si>
     <t>对上游触发重试并在backoff规则内的数量</t>
+  </si>
+  <si>
+    <t>元数据，用于与其他指标联合使用，减少重复字段</t>
+  </si>
+  <si>
+    <t>资源(CPU和内存)使用情况</t>
+  </si>
+  <si>
+    <t>带宽使用情况</t>
+  </si>
+  <si>
+    <t>7层HTTP请求的延迟情况</t>
   </si>
 </sst>
 </file>
@@ -377,6 +389,17 @@
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -386,10 +409,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -399,13 +418,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,38 +734,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED48B81-2504-5D49-9166-2BE7A0090E3A}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B11"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -770,7 +782,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -787,10 +799,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="6" t="s">
         <v>77</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -804,10 +816,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="6" t="s">
         <v>78</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -821,7 +833,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -834,7 +846,7 @@
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -847,11 +859,13 @@
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -862,9 +876,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
       <c r="D9" s="1" t="s">
         <v>32</v>
       </c>
@@ -873,9 +887,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
       <c r="D10" s="1" t="s">
         <v>33</v>
       </c>
@@ -884,9 +898,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
       <c r="D11" s="1" t="s">
         <v>34</v>
       </c>
@@ -895,11 +909,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2" t="s">
+      <c r="B12" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -910,9 +926,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
       <c r="D13" s="1" t="s">
         <v>32</v>
       </c>
@@ -921,9 +937,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
       <c r="D14" s="1" t="s">
         <v>33</v>
       </c>
@@ -932,9 +948,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
       <c r="D15" s="1" t="s">
         <v>35</v>
       </c>
@@ -943,9 +959,9 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
       <c r="D16" s="1" t="s">
         <v>36</v>
       </c>
@@ -954,13 +970,13 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -971,9 +987,9 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
       <c r="D18" s="1" t="s">
         <v>37</v>
       </c>
@@ -982,9 +998,9 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
       <c r="D19" s="1" t="s">
         <v>38</v>
       </c>
@@ -993,9 +1009,9 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
       <c r="D20" s="1" t="s">
         <v>39</v>
       </c>
@@ -1004,9 +1020,9 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="8"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
       <c r="D21" s="1" t="s">
         <v>40</v>
       </c>
@@ -1015,9 +1031,9 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
       <c r="D22" s="1" t="s">
         <v>41</v>
       </c>
@@ -1026,9 +1042,9 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
       <c r="D23" s="1" t="s">
         <v>42</v>
       </c>
@@ -1037,11 +1053,13 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2" t="s">
+      <c r="B24" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -1052,9 +1070,9 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="8"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
       <c r="D25" s="1" t="s">
         <v>36</v>
       </c>
@@ -1063,9 +1081,9 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
       <c r="D26" s="1" t="s">
         <v>38</v>
       </c>
@@ -1074,9 +1092,9 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="8"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
       <c r="D27" s="1" t="s">
         <v>41</v>
       </c>
@@ -1085,9 +1103,9 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="9"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
       <c r="D28" s="1" t="s">
         <v>42</v>
       </c>
@@ -1096,26 +1114,26 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -1126,13 +1144,13 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1143,9 +1161,9 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="8"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
       <c r="D32" s="1" t="s">
         <v>44</v>
       </c>
@@ -1154,9 +1172,9 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="8"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
       <c r="D33" s="1" t="s">
         <v>45</v>
       </c>
@@ -1165,9 +1183,9 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
       <c r="D34" s="1" t="s">
         <v>36</v>
       </c>
@@ -1176,9 +1194,9 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="8"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
       <c r="D35" s="1" t="s">
         <v>46</v>
       </c>
@@ -1187,9 +1205,9 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="9"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
       <c r="D36" s="1" t="s">
         <v>47</v>
       </c>
@@ -1198,11 +1216,13 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2" t="s">
+      <c r="B37" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -1213,9 +1233,9 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
       <c r="D38" s="1" t="s">
         <v>38</v>
       </c>
@@ -1224,9 +1244,9 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="8"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
       <c r="D39" s="1" t="s">
         <v>41</v>
       </c>
@@ -1235,9 +1255,9 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="8"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
       <c r="D40" s="1" t="s">
         <v>36</v>
       </c>
@@ -1246,9 +1266,9 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="9"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
       <c r="D41" s="1" t="s">
         <v>42</v>
       </c>
@@ -1257,13 +1277,13 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -1274,13 +1294,13 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -1291,13 +1311,13 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -1308,13 +1328,13 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -1326,24 +1346,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="C37:C41"/>
+    <mergeCell ref="C31:C36"/>
+    <mergeCell ref="C24:C28"/>
     <mergeCell ref="C8:C11"/>
     <mergeCell ref="C12:C16"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="B17:B23"/>
     <mergeCell ref="B24:B28"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="B37:B41"/>
-    <mergeCell ref="C37:C41"/>
-    <mergeCell ref="C31:C36"/>
-    <mergeCell ref="C24:C28"/>
     <mergeCell ref="C17:C23"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="B8:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>